<commit_message>
Evaluations: #3, finished analyzing video 4
</commit_message>
<xml_diff>
--- a/eval/e3/events.xlsx
+++ b/eval/e3/events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="84">
   <si>
     <t>VidID</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Device|3.7" FWVGA slider</t>
+  </si>
+  <si>
+    <t>Android Device Chooser</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="00"/>
+    <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -344,7 +347,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="21">
@@ -697,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -3169,6 +3172,12 @@
       </c>
     </row>
     <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" t="s">
+        <v>11</v>
+      </c>
       <c r="C107" t="s">
         <v>18</v>
       </c>
@@ -3186,6 +3195,12 @@
       </c>
     </row>
     <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" t="s">
+        <v>11</v>
+      </c>
       <c r="C108" t="s">
         <v>18</v>
       </c>
@@ -3203,6 +3218,12 @@
       </c>
     </row>
     <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
       <c r="C109" t="s">
         <v>18</v>
       </c>
@@ -3220,6 +3241,12 @@
       </c>
     </row>
     <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
       <c r="C110" t="s">
         <v>18</v>
       </c>
@@ -3237,6 +3264,12 @@
       </c>
     </row>
     <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
       <c r="C111" t="s">
         <v>18</v>
       </c>
@@ -3254,6 +3287,12 @@
       </c>
     </row>
     <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
       <c r="C112" t="s">
         <v>18</v>
       </c>
@@ -3270,7 +3309,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="3:7">
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" t="s">
+        <v>11</v>
+      </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
@@ -3287,7 +3332,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="3:7">
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" t="s">
+        <v>11</v>
+      </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
@@ -3304,7 +3355,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="3:7">
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" t="s">
+        <v>11</v>
+      </c>
       <c r="C115" t="s">
         <v>14</v>
       </c>
@@ -3321,7 +3378,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="3:7">
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>79</v>
+      </c>
+      <c r="B116" t="s">
+        <v>11</v>
+      </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
@@ -3338,7 +3401,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="3:7">
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>79</v>
+      </c>
+      <c r="B117" t="s">
+        <v>11</v>
+      </c>
       <c r="C117" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3424,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="3:7">
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" t="s">
+        <v>11</v>
+      </c>
       <c r="C118" t="s">
         <v>14</v>
       </c>
@@ -3370,6 +3445,52 @@
       </c>
       <c r="G118" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>79</v>
+      </c>
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119" t="s">
+        <v>13</v>
+      </c>
+      <c r="E119" s="1">
+        <v>21</v>
+      </c>
+      <c r="F119" s="1">
+        <v>15</v>
+      </c>
+      <c r="G119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>79</v>
+      </c>
+      <c r="B120" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="1">
+        <v>22</v>
+      </c>
+      <c r="F120" s="1">
+        <v>14</v>
+      </c>
+      <c r="G120" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>